<commit_message>
small changes to layout
</commit_message>
<xml_diff>
--- a/control_questions.xlsx
+++ b/control_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanbrady/Desktop/LabResearch/EEG_Protocols/AnonComm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolanbrady/Desktop/LabResearch/IndependentStudy/AnonComm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB2E9C26-78E3-1445-8ACF-9B577259E9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2DED1D-2AB6-7E4F-9454-6278859BBC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48960" yWindow="180" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,10 +69,9 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri Light"/>
             <family val="2"/>
-            <scheme val="major"/>
           </rPr>
           <t xml:space="preserve">Values
 </t>
@@ -80,10 +79,9 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri Light"/>
             <family val="2"/>
-            <scheme val="major"/>
           </rPr>
           <t>Each iteration of this loop, a different one of these values will be chosen. This will be the value of the variable named above.</t>
         </r>
@@ -99,20 +97,20 @@
     <t>prompt</t>
   </si>
   <si>
-    <t>Please describe a pen.</t>
+    <t>Please describe what a pen is.</t>
   </si>
   <si>
-    <t>Please describe school.</t>
+    <t>Please describe what a couch is.</t>
   </si>
   <si>
-    <t>Please describe a goal.</t>
+    <t>Please describe what a shoe is.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,21 +125,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
       <b/>
@@ -517,12 +500,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
@@ -538,12 +521,12 @@
     </row>
     <row r="3" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -559,9 +542,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -679,25 +665,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -719,9 +695,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>